<commit_message>
this has been reupload again
</commit_message>
<xml_diff>
--- a/a.xlsx
+++ b/a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIS ARCHIVOS\17 - PROGRAMACION\7 - JAVA PROGRAMMING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015B781C-27B4-4BE7-B05F-C7902E9E5509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CD5920-4AD1-4C24-A9F8-D4BD59539387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{123B14DD-8072-4431-B27A-D49027CC9C24}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7337" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7338" uniqueCount="6">
   <si>
     <t>ACTIVE RECALL TAGS TEMPLATE</t>
   </si>
@@ -49,6 +49,9 @@
   <si>
     <t>ACTIVE RECALL 
 anki</t>
+  </si>
+  <si>
+    <t>aaaa</t>
   </si>
 </sst>
 </file>
@@ -52758,10 +52761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC3C07D-3C35-42D2-A000-904EA1E00F74}">
-  <dimension ref="A1:XFC122"/>
+  <dimension ref="A1:XFC133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53521,6 +53524,11 @@
         <v>01):)ACTIVE_RECALL::2022-04-18     01):)ACTIVE_RECALL::2022-04-22     01):)ACTIVE_RECALL::2022-04-22     01):)ACTIVE_RECALL::2022-04-28     01):)ACTIVE_RECALL::2022-05-13     01):)ACTIVE_RECALL::2022-06-10     01):)ACTIVE_RECALL::2022-07-28     01):)ACTIVE_RECALL::2022-10-08     01):)ACTIVE_RECALL::2023-03-01</v>
       </c>
     </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:R1"/>

</xml_diff>

<commit_message>
this would be the brand changes
</commit_message>
<xml_diff>
--- a/a.xlsx
+++ b/a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIS ARCHIVOS\17 - PROGRAMACION\7 - JAVA PROGRAMMING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CD5920-4AD1-4C24-A9F8-D4BD59539387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75375978-D332-424B-8111-911A5DFE11E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{123B14DD-8072-4431-B27A-D49027CC9C24}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7338" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7339" uniqueCount="7">
   <si>
     <t>ACTIVE RECALL TAGS TEMPLATE</t>
   </si>
@@ -53,12 +53,15 @@
   <si>
     <t>aaaa</t>
   </si>
+  <si>
+    <t xml:space="preserve">the branch changes are made of me </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +122,14 @@
       <b/>
       <i/>
       <sz val="16"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -205,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -250,6 +261,7 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -53524,6 +53536,11 @@
         <v>01):)ACTIVE_RECALL::2022-04-18     01):)ACTIVE_RECALL::2022-04-22     01):)ACTIVE_RECALL::2022-04-22     01):)ACTIVE_RECALL::2022-04-28     01):)ACTIVE_RECALL::2022-05-13     01):)ACTIVE_RECALL::2022-06-10     01):)ACTIVE_RECALL::2022-07-28     01):)ACTIVE_RECALL::2022-10-08     01):)ACTIVE_RECALL::2023-03-01</v>
       </c>
     </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
adding tone green in our table ->> GREEN
</commit_message>
<xml_diff>
--- a/a.xlsx
+++ b/a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIS ARCHIVOS\17 - PROGRAMACION\7 - JAVA PROGRAMMING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CD5920-4AD1-4C24-A9F8-D4BD59539387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D428DDBB-6A5A-4EA0-B275-5A6CECD0ABE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{123B14DD-8072-4431-B27A-D49027CC9C24}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7338" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7337" uniqueCount="5">
   <si>
     <t>ACTIVE RECALL TAGS TEMPLATE</t>
   </si>
@@ -49,9 +49,6 @@
   <si>
     <t>ACTIVE RECALL 
 anki</t>
-  </si>
-  <si>
-    <t>aaaa</t>
   </si>
 </sst>
 </file>
@@ -205,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -250,6 +247,7 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -53525,9 +53523,7 @@
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A133" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>